<commit_message>
Changed colors in Uebersicht.xls
</commit_message>
<xml_diff>
--- a/Übersicht.xlsx
+++ b/Übersicht.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\there\Documents\Arduino\LEX_2018_grenzschicht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jakob/Documents/Studium/LEX_2018_grenzschicht/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AB19CA-604C-4163-A834-355C98A24CC3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="1" xr2:uid="{D37058A1-8F9F-4CFF-A8F3-53273C08BFC5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>Arduino Nr.</t>
   </si>
@@ -94,18 +99,12 @@
     <t>D13</t>
   </si>
   <si>
-    <t xml:space="preserve">orange </t>
-  </si>
-  <si>
     <t>MiSo</t>
   </si>
   <si>
     <t>D12</t>
   </si>
   <si>
-    <t xml:space="preserve">gelb </t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -142,9 +141,6 @@
     <t>A5</t>
   </si>
   <si>
-    <t>braun</t>
-  </si>
-  <si>
     <t>VCC</t>
   </si>
   <si>
@@ -155,12 +151,15 @@
   </si>
   <si>
     <t>Lauras</t>
+  </si>
+  <si>
+    <t>weiß</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,7 +203,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -515,23 +514,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F29B64C-CC00-447D-9F46-92A0DE2D0949}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="21.7265625" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -551,7 +550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -568,7 +567,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -578,21 +577,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7184642-36FB-439B-830B-57096A71CC07}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -603,7 +602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -611,10 +610,10 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -622,11 +621,11 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -634,11 +633,11 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -646,66 +645,66 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -715,43 +714,43 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
         <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -759,68 +758,68 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D38" s="2"/>
     </row>
   </sheetData>

</xml_diff>